<commit_message>
Say Hi to Friend
AI is mostly complete. Pending some tweaks to the database system to
better enable interaction with the AI system and full integration of
Judge scripts

Font issues w/ C# Card Generation Still not resolved...
</commit_message>
<xml_diff>
--- a/Final Fantasty/Assets/Resources/DB/Ingredients.xlsx
+++ b/Final Fantasty/Assets/Resources/DB/Ingredients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
@@ -67,6 +67,9 @@
     <t xml:space="preserve">Picture Location</t>
   </si>
   <si>
+    <t xml:space="preserve">Step Up</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ingredient</t>
   </si>
   <si>
@@ -85,6 +88,9 @@
     <t xml:space="preserve">ING001</t>
   </si>
   <si>
+    <t xml:space="preserve">tomato, heirloom</t>
+  </si>
+  <si>
     <t xml:space="preserve">Heirloom Tomato</t>
   </si>
   <si>
@@ -94,15 +100,15 @@
     <t xml:space="preserve">Overpowering Flavour</t>
   </si>
   <si>
-    <t xml:space="preserve">tomato, heirloom</t>
-  </si>
-  <si>
     <t xml:space="preserve">HeirloomTomato.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">ING002</t>
   </si>
   <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spaghetti</t>
   </si>
   <si>
@@ -121,15 +127,15 @@
     <t xml:space="preserve">ING003</t>
   </si>
   <si>
+    <t xml:space="preserve">spaghetti, moms</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mom's Spaghetti</t>
   </si>
   <si>
     <t xml:space="preserve">Always Ready, Mom's Spaghetti</t>
   </si>
   <si>
-    <t xml:space="preserve">spaghetti, moms</t>
-  </si>
-  <si>
     <t xml:space="preserve">ING004</t>
   </si>
   <si>
@@ -142,7 +148,7 @@
     <t xml:space="preserve">A Seaside Classic</t>
   </si>
   <si>
-    <t xml:space="preserve">spaghettitomato</t>
+    <t xml:space="preserve">spaghetti;tomato</t>
   </si>
   <si>
     <t xml:space="preserve">Marinara.jpg</t>
@@ -275,26 +281,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.5612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.1887755102041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,16 +352,19 @@
       <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>2</v>
@@ -373,27 +385,30 @@
         <v>1</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
@@ -414,30 +429,33 @@
         <v>3</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
@@ -458,30 +476,33 @@
         <v>0</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
@@ -502,27 +523,30 @@
         <v>0</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M5" s="0" t="s">
         <v>35</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -543,21 +567,24 @@
         <v>2</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
@@ -578,27 +605,30 @@
         <v>1</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -619,16 +649,19 @@
         <v>0</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>